<commit_message>
Added more config parameters
</commit_message>
<xml_diff>
--- a/misc/OAEIAnalaysis.xlsx
+++ b/misc/OAEIAnalaysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="22240" tabRatio="500" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OAEI2011" sheetId="5" r:id="rId1"/>
@@ -2351,12 +2351,48 @@
             <c:strRef>
               <c:f>'Library Only'!$B$8:$B$21</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GOMMA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hertuda</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HotMatch</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>IAMA</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>LogMap</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>LogMap-C</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>LogMapLt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MaasMatch</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MapSSS</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ODGOMS</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Optima</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RSDLWB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ServOMap</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ServOMapLt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2366,12 +2402,39 @@
               <c:f>'Library Only'!$C$5:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="1">
+                  <c:v>0.107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.434</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.537</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.465</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.645</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.688</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>0.577</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.717</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.654</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2396,12 +2459,48 @@
             <c:strRef>
               <c:f>'Library Only'!$B$8:$B$21</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GOMMA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hertuda</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HotMatch</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>IAMA</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>LogMap</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>LogMap-C</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>LogMapLt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MaasMatch</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MapSSS</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ODGOMS</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Optima</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RSDLWB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ServOMap</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ServOMapLt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2411,12 +2510,39 @@
               <c:f>'Library Only'!$D$5:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="1">
+                  <c:v>0.652</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.481</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.575</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.644</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>0.776</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.184</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.072</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.619</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.687</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2441,12 +2567,48 @@
             <c:strRef>
               <c:f>'Library Only'!$B$8:$B$21</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GOMMA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hertuda</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HotMatch</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>IAMA</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>LogMap</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>LogMap-C</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>LogMapLt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MaasMatch</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MapSSS</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ODGOMS</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Optima</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RSDLWB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ServOMap</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ServOMapLt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2456,12 +2618,39 @@
               <c:f>'Library Only'!$E$5:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="1">
+                  <c:v>0.184</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.456</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.619</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.608</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.665</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>0.662</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.272</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.117</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.665</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2476,11 +2665,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131939096"/>
-        <c:axId val="-2131454248"/>
+        <c:axId val="-2124992392"/>
+        <c:axId val="-2124989416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131939096"/>
+        <c:axId val="-2124992392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2489,7 +2678,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131454248"/>
+        <c:crossAx val="-2124989416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2497,7 +2686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131454248"/>
+        <c:axId val="-2124989416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2508,13 +2697,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131939096"/>
+        <c:crossAx val="-2124992392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3108,11 +3298,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113841144"/>
-        <c:axId val="-2113838168"/>
+        <c:axId val="-2124713768"/>
+        <c:axId val="-2124710792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113841144"/>
+        <c:axId val="-2124713768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3121,7 +3311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113838168"/>
+        <c:crossAx val="-2124710792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3129,7 +3319,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113838168"/>
+        <c:axId val="-2124710792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3140,7 +3330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113841144"/>
+        <c:crossAx val="-2124713768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3516,11 +3706,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113803944"/>
-        <c:axId val="-2113800968"/>
+        <c:axId val="-2127027496"/>
+        <c:axId val="-2127024520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113803944"/>
+        <c:axId val="-2127027496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3529,7 +3719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113800968"/>
+        <c:crossAx val="-2127024520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3537,7 +3727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113800968"/>
+        <c:axId val="-2127024520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3548,7 +3738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113803944"/>
+        <c:crossAx val="-2127027496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3762,11 +3952,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113757976"/>
-        <c:axId val="-2113755032"/>
+        <c:axId val="-2124150344"/>
+        <c:axId val="-2124147400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113757976"/>
+        <c:axId val="-2124150344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3775,7 +3965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113755032"/>
+        <c:crossAx val="-2124147400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3783,7 +3973,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113755032"/>
+        <c:axId val="-2124147400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3794,7 +3984,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113757976"/>
+        <c:crossAx val="-2124150344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4431,11 +4621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113715048"/>
-        <c:axId val="-2113712072"/>
+        <c:axId val="-2124107464"/>
+        <c:axId val="-2124104488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113715048"/>
+        <c:axId val="-2124107464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4444,7 +4634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113712072"/>
+        <c:crossAx val="-2124104488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4452,7 +4642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113712072"/>
+        <c:axId val="-2124104488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4463,7 +4653,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113715048"/>
+        <c:crossAx val="-2124107464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5109,11 +5299,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113675736"/>
-        <c:axId val="-2113672760"/>
+        <c:axId val="-2124068152"/>
+        <c:axId val="-2124065176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113675736"/>
+        <c:axId val="-2124068152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5122,7 +5312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113672760"/>
+        <c:crossAx val="-2124065176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5130,7 +5320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113672760"/>
+        <c:axId val="-2124065176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5141,7 +5331,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113675736"/>
+        <c:crossAx val="-2124068152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5643,11 +5833,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113637352"/>
-        <c:axId val="-2113634376"/>
+        <c:axId val="-2124686216"/>
+        <c:axId val="-2124683240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113637352"/>
+        <c:axId val="-2124686216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5656,7 +5846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113634376"/>
+        <c:crossAx val="-2124683240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5664,7 +5854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113634376"/>
+        <c:axId val="-2124683240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5675,7 +5865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113637352"/>
+        <c:crossAx val="-2124686216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5734,24 +5924,87 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>'Library Only'!$B$17:$B$27</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>ODGOMS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Optima</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RSDLWB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ServOMap</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ServOMapLt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>StringsAuto</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WeSeEMtch</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>XMap</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>XMapGen</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>XMapSig</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>YAM++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Library Only'!$F$5:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0.625</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>0.522</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.735</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.777</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
+                  <c:v>0.777</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.646</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.698</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.699</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.774</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.031</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.799</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5773,24 +6026,87 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>'Library Only'!$B$17:$B$27</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>ODGOMS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Optima</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RSDLWB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ServOMap</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ServOMapLt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>StringsAuto</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WeSeEMtch</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>XMap</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>XMapGen</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>XMapSig</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>YAM++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Library Only'!$G$5:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0.877</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>0.918</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.041</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.645</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>0.771</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.783</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.188</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.318</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5812,24 +6128,87 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>'Library Only'!$B$17:$B$27</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>ODGOMS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Optima</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RSDLWB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ServOMap</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ServOMapLt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>StringsAuto</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WeSeEMtch</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>XMap</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>XMapGen</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>XMapSig</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>YAM++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Library Only'!$H$5:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0.73</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>0.666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.648</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.078</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.705</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>0.703</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.758</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.739</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.302</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.057</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.455</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5844,11 +6223,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131379016"/>
-        <c:axId val="-2131376040"/>
+        <c:axId val="-2124957816"/>
+        <c:axId val="-2124954840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131379016"/>
+        <c:axId val="-2124957816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5857,7 +6236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131376040"/>
+        <c:crossAx val="-2124954840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5865,7 +6244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131376040"/>
+        <c:axId val="-2124954840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5876,13 +6255,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131379016"/>
+        <c:crossAx val="-2124957816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5937,14 +6317,35 @@
             <c:strRef>
               <c:f>'Library Only'!$B$5:$B$14</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>AML</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AROMA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CODI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GOMMA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hertuda</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>HotMatch</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>IAMA</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>LogMap</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>LogMap-C</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>LogMapLt</c:v>
                 </c:pt>
               </c:strCache>
@@ -5955,14 +6356,17 @@
               <c:f>'Library Only'!$I$5:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.824</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7">
                   <c:v>0.743</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>0.484</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.644</c:v>
                 </c:pt>
               </c:numCache>
@@ -5988,14 +6392,35 @@
             <c:strRef>
               <c:f>'Library Only'!$B$5:$B$14</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>AML</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AROMA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CODI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GOMMA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hertuda</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>HotMatch</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>IAMA</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>LogMap</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>LogMap-C</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>LogMapLt</c:v>
                 </c:pt>
               </c:strCache>
@@ -6006,14 +6431,17 @@
               <c:f>'Library Only'!$J$5:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.778</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7">
                   <c:v>0.681</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>0.264</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.771</c:v>
                 </c:pt>
               </c:numCache>
@@ -6039,14 +6467,35 @@
             <c:strRef>
               <c:f>'Library Only'!$B$5:$B$14</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>AML</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AROMA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CODI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GOMMA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hertuda</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>HotMatch</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>IAMA</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>LogMap</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>LogMap-C</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>LogMapLt</c:v>
                 </c:pt>
               </c:strCache>
@@ -6057,14 +6506,17 @@
               <c:f>'Library Only'!$K$5:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7">
                   <c:v>0.711</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>0.342</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.702</c:v>
                 </c:pt>
               </c:numCache>
@@ -6080,11 +6532,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131344184"/>
-        <c:axId val="-2131341208"/>
+        <c:axId val="-2124922968"/>
+        <c:axId val="-2124919992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131344184"/>
+        <c:axId val="-2124922968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6093,7 +6545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131341208"/>
+        <c:crossAx val="-2124919992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6101,7 +6553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131341208"/>
+        <c:axId val="-2124919992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6112,13 +6564,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131344184"/>
+        <c:crossAx val="-2124922968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6748,11 +7201,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131291832"/>
-        <c:axId val="-2131288856"/>
+        <c:axId val="-2127045272"/>
+        <c:axId val="-2127042296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131291832"/>
+        <c:axId val="-2127045272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6761,7 +7214,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131288856"/>
+        <c:crossAx val="-2127042296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6769,7 +7222,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131288856"/>
+        <c:axId val="-2127042296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6780,13 +7233,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131291832"/>
+        <c:crossAx val="-2127045272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7452,11 +7906,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131898072"/>
-        <c:axId val="-2131895096"/>
+        <c:axId val="-2124893576"/>
+        <c:axId val="-2124890600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131898072"/>
+        <c:axId val="-2124893576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7465,7 +7919,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131895096"/>
+        <c:crossAx val="-2124890600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7473,7 +7927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131895096"/>
+        <c:axId val="-2124890600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7484,13 +7938,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131898072"/>
+        <c:crossAx val="-2124893576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8183,11 +8638,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131858104"/>
-        <c:axId val="-2131855128"/>
+        <c:axId val="-2124853352"/>
+        <c:axId val="-2124850376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131858104"/>
+        <c:axId val="-2124853352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8196,7 +8651,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131855128"/>
+        <c:crossAx val="-2124850376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8204,7 +8659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131855128"/>
+        <c:axId val="-2124850376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8215,13 +8670,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131858104"/>
+        <c:crossAx val="-2124853352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8806,11 +9262,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131817336"/>
-        <c:axId val="-2131814360"/>
+        <c:axId val="-2124208152"/>
+        <c:axId val="-2124205176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131817336"/>
+        <c:axId val="-2124208152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8819,7 +9275,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131814360"/>
+        <c:crossAx val="-2124205176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8827,7 +9283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131814360"/>
+        <c:axId val="-2124205176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8838,7 +9294,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131817336"/>
+        <c:crossAx val="-2124208152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9078,11 +9534,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2132767224"/>
-        <c:axId val="-2132770216"/>
+        <c:axId val="-2124794264"/>
+        <c:axId val="-2124791288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2132767224"/>
+        <c:axId val="-2124794264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9091,7 +9547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132770216"/>
+        <c:crossAx val="-2124791288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9099,7 +9555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132770216"/>
+        <c:axId val="-2124791288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9110,13 +9566,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132767224"/>
+        <c:crossAx val="-2124794264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9647,11 +10104,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113881240"/>
-        <c:axId val="-2113878264"/>
+        <c:axId val="-2124753688"/>
+        <c:axId val="-2124750712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113881240"/>
+        <c:axId val="-2124753688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9660,7 +10117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113878264"/>
+        <c:crossAx val="-2124750712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9668,7 +10125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113878264"/>
+        <c:axId val="-2124750712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9679,7 +10136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113881240"/>
+        <c:crossAx val="-2124753688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14843,11 +15300,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B2:N75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14932,7 +15388,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" hidden="1">
+    <row r="6" spans="2:11">
       <c r="B6" s="88" t="s">
         <v>48</v>
       </c>
@@ -14952,7 +15408,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="23"/>
     </row>
-    <row r="7" spans="2:11" hidden="1">
+    <row r="7" spans="2:11">
       <c r="B7" s="88" t="s">
         <v>51</v>
       </c>
@@ -14972,7 +15428,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="23"/>
     </row>
-    <row r="8" spans="2:11" hidden="1">
+    <row r="8" spans="2:11">
       <c r="B8" s="161" t="s">
         <v>52</v>
       </c>
@@ -14992,7 +15448,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="23"/>
     </row>
-    <row r="9" spans="2:11" hidden="1">
+    <row r="9" spans="2:11">
       <c r="B9" s="88" t="s">
         <v>29</v>
       </c>
@@ -15018,7 +15474,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="23"/>
     </row>
-    <row r="10" spans="2:11" hidden="1">
+    <row r="10" spans="2:11">
       <c r="B10" s="88" t="s">
         <v>30</v>
       </c>
@@ -15044,7 +15500,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="23"/>
     </row>
-    <row r="11" spans="2:11" hidden="1">
+    <row r="11" spans="2:11">
       <c r="B11" s="88" t="s">
         <v>31</v>
       </c>
@@ -15096,7 +15552,7 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="13" spans="2:11" hidden="1">
+    <row r="13" spans="2:11">
       <c r="B13" s="88" t="s">
         <v>7</v>
       </c>
@@ -15148,7 +15604,7 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="15" spans="2:11" hidden="1">
+    <row r="15" spans="2:11">
       <c r="B15" s="88" t="s">
         <v>10</v>
       </c>
@@ -15168,7 +15624,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="16" spans="2:11" hidden="1">
+    <row r="16" spans="2:11">
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -15188,7 +15644,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="2:14" hidden="1">
+    <row r="17" spans="2:14">
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -15208,7 +15664,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="23"/>
     </row>
-    <row r="18" spans="2:14" hidden="1">
+    <row r="18" spans="2:14">
       <c r="B18" s="88" t="s">
         <v>55</v>
       </c>
@@ -15228,7 +15684,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="23"/>
     </row>
-    <row r="19" spans="2:14" hidden="1">
+    <row r="19" spans="2:14">
       <c r="B19" s="72" t="s">
         <v>13</v>
       </c>
@@ -15248,7 +15704,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:14" hidden="1">
+    <row r="20" spans="2:14">
       <c r="B20" s="88" t="s">
         <v>37</v>
       </c>
@@ -15274,7 +15730,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="23"/>
     </row>
-    <row r="21" spans="2:14" hidden="1">
+    <row r="21" spans="2:14">
       <c r="B21" s="162" t="s">
         <v>56</v>
       </c>
@@ -15294,7 +15750,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="23"/>
     </row>
-    <row r="22" spans="2:14" hidden="1">
+    <row r="22" spans="2:14">
       <c r="B22" s="49" t="s">
         <v>38</v>
       </c>
@@ -15314,7 +15770,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="23"/>
     </row>
-    <row r="23" spans="2:14" hidden="1">
+    <row r="23" spans="2:14">
       <c r="B23" s="90" t="s">
         <v>58</v>
       </c>
@@ -15334,7 +15790,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="23"/>
     </row>
-    <row r="24" spans="2:14" hidden="1">
+    <row r="24" spans="2:14">
       <c r="B24" s="49" t="s">
         <v>14</v>
       </c>
@@ -15354,7 +15810,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="25" spans="2:14" hidden="1">
+    <row r="25" spans="2:14">
       <c r="B25" s="49" t="s">
         <v>43</v>
       </c>
@@ -15374,7 +15830,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="23"/>
     </row>
-    <row r="26" spans="2:14" hidden="1">
+    <row r="26" spans="2:14">
       <c r="B26" s="49" t="s">
         <v>44</v>
       </c>
@@ -15394,7 +15850,7 @@
       <c r="J26" s="101"/>
       <c r="K26" s="102"/>
     </row>
-    <row r="27" spans="2:14" ht="16" hidden="1" thickBot="1">
+    <row r="27" spans="2:14" ht="16" thickBot="1">
       <c r="B27" s="91" t="s">
         <v>42</v>
       </c>
@@ -15536,11 +15992,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B4:K27">
-    <filterColumn colId="9">
-      <top10 val="3" filterVal="0.70199999999999996"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B4:K27"/>
   <sortState ref="B5:K30">
     <sortCondition ref="B5"/>
   </sortState>
@@ -15560,10 +16012,10 @@
   <dimension ref="B3:N108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B47" sqref="B47:N50"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7:N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16839,8 +17291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N105"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6:N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17924,7 +18376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:N116"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -19141,8 +19593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>